<commit_message>
Code Organizing / AT4 Buff
The AT4 was kinda too shit and organized some enemy code so isn't all jenk looking
</commit_message>
<xml_diff>
--- a/Map 1 Assets/Map 1 - Gun Damage, Explosive, and Trap Values Values.xlsx
+++ b/Map 1 Assets/Map 1 - Gun Damage, Explosive, and Trap Values Values.xlsx
@@ -314,9 +314,6 @@
     <t>1 Frame/ 35,70,105,140  Up 50,85,120,135</t>
   </si>
   <si>
-    <t>1 Frame / 35,70,105,140 Up 50,85,120,155</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.5 Frames </t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t xml:space="preserve">90 Frames </t>
+  </si>
+  <si>
+    <t>1 Frame / 35,70,105,140,175 Up 50,85,120,155,190</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
     <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1105,16 +1105,16 @@
         <v>10</v>
       </c>
       <c r="D15" s="2">
-        <v>225190155120</v>
+        <v>325290255220195</v>
       </c>
       <c r="E15" s="2">
-        <v>275240205165</v>
+        <v>375340305265230</v>
       </c>
       <c r="F15" t="s">
         <v>65</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H15" t="s">
         <v>80</v>
@@ -1172,7 +1172,7 @@
         <v>45</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17" t="s">
         <v>84</v>
@@ -1230,7 +1230,7 @@
         <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" t="s">
         <v>85</v>
@@ -1288,7 +1288,7 @@
         <v>46</v>
       </c>
       <c r="G21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
         <v>80</v>

</xml_diff>